<commit_message>
updated test triplet controls file column header
</commit_message>
<xml_diff>
--- a/Triplet_controls.xlsx
+++ b/Triplet_controls.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Gene1</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>33/25</t>
+  </si>
+  <si>
+    <t>reference_sample</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -415,6 +418,9 @@
     <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
update tester triplet controls.xlsx
</commit_message>
<xml_diff>
--- a/Triplet_controls.xlsx
+++ b/Triplet_controls.xlsx
@@ -48,34 +48,34 @@
     <t>289/376</t>
   </si>
   <si>
+    <t>305/284</t>
+  </si>
+  <si>
+    <t>Exp_peaks</t>
+  </si>
+  <si>
+    <t>Exp_repeats</t>
+  </si>
+  <si>
+    <t>30/51</t>
+  </si>
+  <si>
+    <t>35/29</t>
+  </si>
+  <si>
+    <t>reference_sample</t>
+  </si>
+  <si>
     <t>297/323</t>
   </si>
   <si>
-    <t>297/276</t>
-  </si>
-  <si>
-    <t>305/284</t>
-  </si>
-  <si>
-    <t>Exp_peaks</t>
-  </si>
-  <si>
-    <t>Exp_repeats</t>
-  </si>
-  <si>
-    <t>30/51</t>
+    <t>294/276</t>
   </si>
   <si>
     <t>33/45</t>
   </si>
   <si>
-    <t>35/29</t>
-  </si>
-  <si>
-    <t>33/25</t>
-  </si>
-  <si>
-    <t>reference_sample</t>
+    <t>32/25</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -420,13 +420,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -449,7 +449,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -457,10 +457,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -468,10 +468,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -479,10 +479,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>